<commit_message>
small updates in report template
</commit_message>
<xml_diff>
--- a/spreadsheets/menu_report.xlsx
+++ b/spreadsheets/menu_report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ЦяКнига" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="19440" windowHeight="13875"/>
@@ -10,7 +10,7 @@
     <sheet name="Меню" sheetId="4" r:id="rId1"/>
     <sheet name="Вимога" sheetId="5" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -38,12 +38,6 @@
     <t>МЕНЮ-РОЗКЛАДКА</t>
   </si>
   <si>
-    <t>реабілітації дітей-інвалідів"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">"Вараський міський центр соціальної </t>
-  </si>
-  <si>
     <t>Директор комунального закладу</t>
   </si>
   <si>
@@ -135,6 +129,12 @@
   </si>
   <si>
     <t>{first_issued_header}</t>
+  </si>
+  <si>
+    <t>"Вараський міський центр комплексної</t>
+  </si>
+  <si>
+    <t>реабілітації для осіб з інвалідністю"</t>
   </si>
 </sst>
 </file>
@@ -594,88 +594,88 @@
     <xf numFmtId="2" fontId="30" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="25" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="25" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -694,7 +694,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Стандартна">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -732,7 +732,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Стандартна">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -804,7 +804,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Стандартна">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1017,7 +1017,7 @@
       <c r="J1" s="16"/>
       <c r="K1" s="15"/>
       <c r="L1" s="27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M1" s="27"/>
       <c r="N1" s="27"/>
@@ -1038,7 +1038,7 @@
       <c r="J2" s="16"/>
       <c r="K2" s="15"/>
       <c r="L2" s="27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M2" s="27"/>
       <c r="N2" s="27"/>
@@ -1059,7 +1059,7 @@
       <c r="J3" s="16"/>
       <c r="K3" s="15"/>
       <c r="L3" s="28" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="M3" s="29"/>
       <c r="N3" s="29"/>
@@ -1080,7 +1080,7 @@
       <c r="J4" s="16"/>
       <c r="K4" s="15"/>
       <c r="L4" s="27" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="M4" s="27"/>
       <c r="N4" s="27"/>
@@ -1101,7 +1101,7 @@
       <c r="J5" s="16"/>
       <c r="K5" s="15"/>
       <c r="L5" s="30" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M5" s="30"/>
       <c r="N5" s="30"/>
@@ -1125,7 +1125,7 @@
       <c r="M6" s="32"/>
       <c r="N6" s="32"/>
       <c r="O6" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="P6" s="27"/>
       <c r="Q6" s="17"/>
@@ -1143,7 +1143,7 @@
       <c r="J7" s="16"/>
       <c r="K7" s="15"/>
       <c r="L7" s="33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="M7" s="33"/>
       <c r="N7" s="33"/>
@@ -1152,46 +1152,46 @@
       <c r="Q7" s="18"/>
     </row>
     <row r="8" spans="1:17" s="10" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="83" t="s">
+      <c r="A8" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="83"/>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
-      <c r="F8" s="83"/>
-      <c r="G8" s="83"/>
-      <c r="H8" s="83"/>
-      <c r="I8" s="83"/>
-      <c r="J8" s="83"/>
-      <c r="K8" s="83"/>
-      <c r="L8" s="83"/>
-      <c r="M8" s="83"/>
-      <c r="N8" s="83"/>
-      <c r="O8" s="83"/>
-      <c r="P8" s="83"/>
-      <c r="Q8" s="83"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="81"/>
+      <c r="D8" s="81"/>
+      <c r="E8" s="81"/>
+      <c r="F8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="81"/>
+      <c r="J8" s="81"/>
+      <c r="K8" s="81"/>
+      <c r="L8" s="81"/>
+      <c r="M8" s="81"/>
+      <c r="N8" s="81"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="81"/>
+      <c r="Q8" s="81"/>
     </row>
     <row r="9" spans="1:17" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="86" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="86"/>
+      <c r="A9" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="88"/>
+      <c r="C9" s="88"/>
+      <c r="D9" s="88"/>
+      <c r="E9" s="88"/>
+      <c r="F9" s="88"/>
+      <c r="G9" s="88"/>
+      <c r="H9" s="88"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="88"/>
+      <c r="K9" s="88"/>
+      <c r="L9" s="88"/>
+      <c r="M9" s="88"/>
+      <c r="N9" s="88"/>
+      <c r="O9" s="88"/>
+      <c r="P9" s="88"/>
+      <c r="Q9" s="88"/>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
@@ -1224,14 +1224,14 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="85" t="s">
-        <v>26</v>
-      </c>
-      <c r="M11" s="85"/>
-      <c r="N11" s="85"/>
-      <c r="O11" s="85"/>
-      <c r="P11" s="85"/>
-      <c r="Q11" s="85"/>
+      <c r="L11" s="87" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="87"/>
+      <c r="N11" s="87"/>
+      <c r="O11" s="87"/>
+      <c r="P11" s="87"/>
+      <c r="Q11" s="87"/>
     </row>
     <row r="12" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
@@ -1245,17 +1245,17 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="84" t="s">
+      <c r="L12" s="82" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="84"/>
-      <c r="N12" s="84"/>
-      <c r="O12" s="81">
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="86">
         <f>SUM(O13:Q17)</f>
         <v>0</v>
       </c>
-      <c r="P12" s="82"/>
-      <c r="Q12" s="82"/>
+      <c r="P12" s="89"/>
+      <c r="Q12" s="89"/>
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
@@ -1269,16 +1269,16 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="77" t="s">
-        <v>32</v>
-      </c>
-      <c r="M13" s="78"/>
-      <c r="N13" s="79"/>
-      <c r="O13" s="81" t="s">
-        <v>33</v>
-      </c>
-      <c r="P13" s="82"/>
-      <c r="Q13" s="82"/>
+      <c r="L13" s="83" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="84"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="86" t="s">
+        <v>31</v>
+      </c>
+      <c r="P13" s="89"/>
+      <c r="Q13" s="89"/>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
@@ -1292,12 +1292,12 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="77"/>
-      <c r="M14" s="78"/>
-      <c r="N14" s="79"/>
-      <c r="O14" s="81"/>
-      <c r="P14" s="81"/>
-      <c r="Q14" s="81"/>
+      <c r="L14" s="83"/>
+      <c r="M14" s="84"/>
+      <c r="N14" s="85"/>
+      <c r="O14" s="86"/>
+      <c r="P14" s="86"/>
+      <c r="Q14" s="86"/>
     </row>
     <row r="15" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
@@ -1311,12 +1311,12 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="77"/>
-      <c r="M15" s="78"/>
-      <c r="N15" s="79"/>
-      <c r="O15" s="81"/>
-      <c r="P15" s="81"/>
-      <c r="Q15" s="81"/>
+      <c r="L15" s="83"/>
+      <c r="M15" s="84"/>
+      <c r="N15" s="85"/>
+      <c r="O15" s="86"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="86"/>
     </row>
     <row r="16" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
@@ -1330,12 +1330,12 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
-      <c r="O16" s="81"/>
-      <c r="P16" s="81"/>
-      <c r="Q16" s="81"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="86"/>
+      <c r="N16" s="86"/>
+      <c r="O16" s="86"/>
+      <c r="P16" s="86"/>
+      <c r="Q16" s="86"/>
     </row>
     <row r="17" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
@@ -1349,12 +1349,12 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="77"/>
-      <c r="M17" s="78"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="81"/>
-      <c r="P17" s="81"/>
-      <c r="Q17" s="81"/>
+      <c r="L17" s="83"/>
+      <c r="M17" s="84"/>
+      <c r="N17" s="85"/>
+      <c r="O17" s="86"/>
+      <c r="P17" s="86"/>
+      <c r="Q17" s="86"/>
     </row>
     <row r="18" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
@@ -1376,50 +1376,50 @@
       <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="80" t="s">
+      <c r="A19" s="90" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="84" t="s">
+      <c r="B19" s="82" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84" t="s">
+      <c r="C19" s="82"/>
+      <c r="D19" s="82"/>
+      <c r="E19" s="82"/>
+      <c r="F19" s="82"/>
+      <c r="G19" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84" t="s">
+      <c r="H19" s="82"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="82" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="84"/>
-      <c r="N19" s="84"/>
-      <c r="O19" s="84"/>
-      <c r="P19" s="84"/>
-      <c r="Q19" s="84"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="82"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="82"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="80"/>
+      <c r="A20" s="90"/>
       <c r="B20" s="24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="24"/>
       <c r="D20" s="24"/>
       <c r="E20" s="24"/>
       <c r="F20" s="24"/>
       <c r="G20" s="24" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H20" s="24"/>
       <c r="I20" s="24"/>
       <c r="J20" s="24"/>
       <c r="K20" s="24"/>
       <c r="L20" s="24" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="M20" s="24"/>
       <c r="N20" s="24"/>
@@ -1431,7 +1431,7 @@
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="65" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B21" s="66"/>
       <c r="C21" s="66"/>
@@ -1472,13 +1472,13 @@
     <row r="23" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="21"/>
       <c r="C23" s="67" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D23" s="23"/>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
       <c r="G23" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H23" s="11"/>
       <c r="I23" s="5"/>
@@ -1493,9 +1493,9 @@
     </row>
     <row r="24" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
-      <c r="D24" s="105"/>
-      <c r="E24" s="105"/>
-      <c r="F24" s="105"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -1511,17 +1511,20 @@
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D25" s="77"/>
+      <c r="E25" s="78"/>
+      <c r="F25" s="79"/>
+      <c r="G25" s="22" t="s">
         <v>28</v>
-      </c>
-      <c r="D25" s="102"/>
-      <c r="E25" s="103"/>
-      <c r="F25" s="104"/>
-      <c r="G25" s="22" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="L16:N16"/>
     <mergeCell ref="A8:Q8"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="L17:N17"/>
@@ -1538,9 +1541,6 @@
     <mergeCell ref="L14:N14"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="L16:N16"/>
   </mergeCells>
   <pageMargins left="0.56000000000000005" right="0.37" top="0.62" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1553,7 +1553,7 @@
   <dimension ref="A1:AP26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1570,7 +1570,7 @@
   <sheetData>
     <row r="1" spans="1:42" s="42" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M1" s="27" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="N1" s="12"/>
       <c r="O1" s="12"/>
@@ -1581,12 +1581,12 @@
       <c r="T1" s="16"/>
       <c r="U1" s="43"/>
       <c r="V1" s="43"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
+      <c r="W1" s="100"/>
+      <c r="X1" s="100"/>
+      <c r="Y1" s="100"/>
+      <c r="Z1" s="100"/>
+      <c r="AA1" s="100"/>
+      <c r="AB1" s="100"/>
       <c r="AC1" s="26"/>
       <c r="AD1" s="17"/>
       <c r="AE1" s="44"/>
@@ -1598,7 +1598,7 @@
     </row>
     <row r="2" spans="1:42" s="42" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M2" s="27" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="N2" s="47"/>
       <c r="O2" s="47"/>
@@ -1609,14 +1609,14 @@
       <c r="T2" s="47"/>
       <c r="U2" s="43"/>
       <c r="V2" s="43"/>
-      <c r="W2" s="87"/>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87"/>
-      <c r="Z2" s="87"/>
-      <c r="AA2" s="87"/>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="87"/>
-      <c r="AD2" s="87"/>
+      <c r="W2" s="100"/>
+      <c r="X2" s="100"/>
+      <c r="Y2" s="100"/>
+      <c r="Z2" s="100"/>
+      <c r="AA2" s="100"/>
+      <c r="AB2" s="100"/>
+      <c r="AC2" s="100"/>
+      <c r="AD2" s="100"/>
       <c r="AE2" s="44"/>
       <c r="AF2" s="44"/>
       <c r="AG2" s="44"/>
@@ -1626,7 +1626,7 @@
     </row>
     <row r="3" spans="1:42" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M3" s="28" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="N3" s="13"/>
       <c r="O3" s="13"/>
@@ -1637,14 +1637,14 @@
       <c r="T3" s="13"/>
       <c r="U3" s="43"/>
       <c r="V3" s="43"/>
-      <c r="W3" s="88"/>
-      <c r="X3" s="88"/>
-      <c r="Y3" s="88"/>
-      <c r="Z3" s="88"/>
-      <c r="AA3" s="88"/>
-      <c r="AB3" s="88"/>
-      <c r="AC3" s="88"/>
-      <c r="AD3" s="88"/>
+      <c r="W3" s="101"/>
+      <c r="X3" s="101"/>
+      <c r="Y3" s="101"/>
+      <c r="Z3" s="101"/>
+      <c r="AA3" s="101"/>
+      <c r="AB3" s="101"/>
+      <c r="AC3" s="101"/>
+      <c r="AD3" s="101"/>
       <c r="AE3" s="48"/>
       <c r="AF3" s="48"/>
       <c r="AG3" s="48"/>
@@ -1654,7 +1654,7 @@
     </row>
     <row r="4" spans="1:42" s="42" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M4" s="27" t="s">
-        <v>7</v>
+        <v>39</v>
       </c>
       <c r="N4" s="12"/>
       <c r="O4" s="12"/>
@@ -1665,13 +1665,13 @@
       <c r="T4" s="15"/>
       <c r="U4" s="43"/>
       <c r="V4" s="43"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="87"/>
+      <c r="W4" s="100"/>
+      <c r="X4" s="100"/>
+      <c r="Y4" s="100"/>
+      <c r="Z4" s="100"/>
+      <c r="AA4" s="100"/>
+      <c r="AB4" s="100"/>
+      <c r="AC4" s="100"/>
       <c r="AD4" s="26"/>
       <c r="AE4" s="48"/>
       <c r="AF4" s="48"/>
@@ -1682,23 +1682,23 @@
     </row>
     <row r="5" spans="1:42" s="42" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M5" s="30" t="s">
-        <v>21</v>
-      </c>
-      <c r="T5" s="90"/>
-      <c r="U5" s="90"/>
-      <c r="V5" s="90"/>
-      <c r="W5" s="90"/>
-      <c r="X5" s="90"/>
-      <c r="Y5" s="90"/>
+        <v>19</v>
+      </c>
+      <c r="T5" s="103"/>
+      <c r="U5" s="103"/>
+      <c r="V5" s="103"/>
+      <c r="W5" s="103"/>
+      <c r="X5" s="103"/>
+      <c r="Y5" s="103"/>
       <c r="Z5" s="18"/>
       <c r="AB5" s="43"/>
       <c r="AC5" s="43"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="91"/>
-      <c r="AF5" s="91"/>
-      <c r="AG5" s="91"/>
-      <c r="AH5" s="91"/>
-      <c r="AI5" s="91"/>
+      <c r="AD5" s="104"/>
+      <c r="AE5" s="104"/>
+      <c r="AF5" s="104"/>
+      <c r="AG5" s="104"/>
+      <c r="AH5" s="104"/>
+      <c r="AI5" s="104"/>
       <c r="AJ5" s="18"/>
     </row>
     <row r="6" spans="1:42" s="42" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1706,7 +1706,7 @@
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
       <c r="P6" s="27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Q6" s="12"/>
       <c r="R6" s="12"/>
@@ -1735,7 +1735,7 @@
     </row>
     <row r="7" spans="1:42" s="42" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="M7" s="33" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="N7" s="20"/>
       <c r="O7" s="20"/>
@@ -1764,67 +1764,67 @@
       <c r="AN7" s="54"/>
     </row>
     <row r="8" spans="1:42" s="55" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="92" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="92"/>
-      <c r="O8" s="92"/>
-      <c r="P8" s="92"/>
-      <c r="Q8" s="92"/>
+      <c r="A8" s="105" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="105"/>
+      <c r="C8" s="105"/>
+      <c r="D8" s="105"/>
+      <c r="E8" s="105"/>
+      <c r="F8" s="105"/>
+      <c r="G8" s="105"/>
+      <c r="H8" s="105"/>
+      <c r="I8" s="105"/>
+      <c r="J8" s="105"/>
+      <c r="K8" s="105"/>
+      <c r="L8" s="105"/>
+      <c r="M8" s="105"/>
+      <c r="N8" s="105"/>
+      <c r="O8" s="105"/>
+      <c r="P8" s="105"/>
+      <c r="Q8" s="105"/>
     </row>
     <row r="9" spans="1:42" s="56" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="89" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="89"/>
-      <c r="M9" s="89"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="89"/>
-      <c r="P9" s="89"/>
-      <c r="Q9" s="89"/>
+      <c r="A9" s="102" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="102"/>
+      <c r="C9" s="102"/>
+      <c r="D9" s="102"/>
+      <c r="E9" s="102"/>
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="102"/>
+      <c r="J9" s="102"/>
+      <c r="K9" s="102"/>
+      <c r="L9" s="102"/>
+      <c r="M9" s="102"/>
+      <c r="N9" s="102"/>
+      <c r="O9" s="102"/>
+      <c r="P9" s="102"/>
+      <c r="Q9" s="102"/>
     </row>
     <row r="10" spans="1:42" s="56" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A10" s="86" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="86"/>
-      <c r="Q10" s="86"/>
+      <c r="A10" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
+      <c r="F10" s="88"/>
+      <c r="G10" s="88"/>
+      <c r="H10" s="88"/>
+      <c r="I10" s="88"/>
+      <c r="J10" s="88"/>
+      <c r="K10" s="88"/>
+      <c r="L10" s="88"/>
+      <c r="M10" s="88"/>
+      <c r="N10" s="88"/>
+      <c r="O10" s="88"/>
+      <c r="P10" s="88"/>
+      <c r="Q10" s="88"/>
     </row>
     <row r="11" spans="1:42" s="42" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A11" s="57"/>
@@ -1843,47 +1843,47 @@
       <c r="O11" s="58"/>
       <c r="P11" s="58"/>
       <c r="Q11" s="59" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:42" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="100" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="95" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="93" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="95" t="s">
+      <c r="A12" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="97" t="s">
+      <c r="B12" s="93" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="91" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="93" t="s">
+      <c r="D12" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="M12" s="93"/>
-      <c r="N12" s="93"/>
-      <c r="O12" s="93"/>
-      <c r="P12" s="93"/>
-      <c r="Q12" s="93"/>
+      <c r="E12" s="95" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="96"/>
+      <c r="G12" s="96"/>
+      <c r="H12" s="96"/>
+      <c r="I12" s="96"/>
+      <c r="J12" s="96"/>
+      <c r="K12" s="97"/>
+      <c r="L12" s="91" t="s">
+        <v>12</v>
+      </c>
+      <c r="M12" s="91"/>
+      <c r="N12" s="91"/>
+      <c r="O12" s="91"/>
+      <c r="P12" s="91"/>
+      <c r="Q12" s="91"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A13" s="101"/>
-      <c r="B13" s="96"/>
-      <c r="C13" s="94"/>
-      <c r="D13" s="96"/>
+      <c r="A13" s="99"/>
+      <c r="B13" s="94"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="94"/>
       <c r="E13" s="34" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F13" s="34"/>
       <c r="G13" s="34"/>
@@ -1893,10 +1893,10 @@
         <v>0</v>
       </c>
       <c r="K13" s="34" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="L13" s="34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
@@ -1908,7 +1908,7 @@
     </row>
     <row r="14" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="72" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B14" s="72"/>
       <c r="C14" s="73"/>
@@ -1968,12 +1968,12 @@
     <row r="17" spans="2:7" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="70"/>
       <c r="C17" s="69" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D17" s="37"/>
       <c r="E17" s="37"/>
       <c r="F17" s="38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G17" s="35"/>
     </row>
@@ -1984,7 +1984,7 @@
     </row>
     <row r="19" spans="2:7" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C19" s="68" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D19" s="39"/>
       <c r="E19" s="40"/>
@@ -1998,12 +1998,6 @@
     <row r="26" spans="2:7" s="42" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="L12:Q12"/>
-    <mergeCell ref="E12:K12"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="W1:AB1"/>
     <mergeCell ref="W2:AD2"/>
     <mergeCell ref="W3:AD3"/>
@@ -2013,6 +2007,12 @@
     <mergeCell ref="AD5:AI5"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="A8:Q8"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="L12:Q12"/>
+    <mergeCell ref="E12:K12"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.31496062992125984" top="0.78740157480314965" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="83" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
duplicate the table of demand
</commit_message>
<xml_diff>
--- a/spreadsheets/menu_report.xlsx
+++ b/spreadsheets/menu_report.xlsx
@@ -446,7 +446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="104">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -492,23 +492,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -528,21 +511,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -553,31 +521,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="2" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -586,6 +529,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -594,6 +540,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -614,51 +563,99 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1138,46 +1135,46 @@
       <c r="Q7" s="18"/>
     </row>
     <row r="8" spans="1:17" s="10" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="84" t="s">
+      <c r="A8" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="84"/>
-      <c r="N8" s="84"/>
-      <c r="O8" s="84"/>
-      <c r="P8" s="84"/>
-      <c r="Q8" s="84"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="59"/>
+      <c r="F8" s="59"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="59"/>
+      <c r="N8" s="59"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="59"/>
+      <c r="Q8" s="59"/>
     </row>
     <row r="9" spans="1:17" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="86" t="s">
+      <c r="A9" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="86"/>
-      <c r="C9" s="86"/>
-      <c r="D9" s="86"/>
-      <c r="E9" s="86"/>
-      <c r="F9" s="86"/>
-      <c r="G9" s="86"/>
-      <c r="H9" s="86"/>
-      <c r="I9" s="86"/>
-      <c r="J9" s="86"/>
-      <c r="K9" s="86"/>
-      <c r="L9" s="86"/>
-      <c r="M9" s="86"/>
-      <c r="N9" s="86"/>
-      <c r="O9" s="86"/>
-      <c r="P9" s="86"/>
-      <c r="Q9" s="86"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="61"/>
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="N9" s="61"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
@@ -1210,14 +1207,14 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="85" t="s">
+      <c r="L11" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="85"/>
-      <c r="N11" s="85"/>
-      <c r="O11" s="85"/>
-      <c r="P11" s="85"/>
-      <c r="Q11" s="85"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="60"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="60"/>
     </row>
     <row r="12" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
@@ -1231,17 +1228,17 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="82" t="s">
+      <c r="L12" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="82"/>
-      <c r="N12" s="82"/>
-      <c r="O12" s="82">
+      <c r="M12" s="57"/>
+      <c r="N12" s="57"/>
+      <c r="O12" s="57">
         <f>SUM(O13:Q17)</f>
         <v>0</v>
       </c>
-      <c r="P12" s="83"/>
-      <c r="Q12" s="83"/>
+      <c r="P12" s="58"/>
+      <c r="Q12" s="58"/>
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
@@ -1255,16 +1252,16 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="79" t="s">
+      <c r="L13" s="53" t="s">
         <v>29</v>
       </c>
-      <c r="M13" s="80"/>
-      <c r="N13" s="81"/>
-      <c r="O13" s="82" t="s">
+      <c r="M13" s="54"/>
+      <c r="N13" s="55"/>
+      <c r="O13" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="P13" s="83"/>
-      <c r="Q13" s="83"/>
+      <c r="P13" s="58"/>
+      <c r="Q13" s="58"/>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
@@ -1278,12 +1275,12 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="79"/>
-      <c r="M14" s="80"/>
-      <c r="N14" s="81"/>
-      <c r="O14" s="82"/>
-      <c r="P14" s="82"/>
-      <c r="Q14" s="82"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="54"/>
+      <c r="N14" s="55"/>
+      <c r="O14" s="57"/>
+      <c r="P14" s="57"/>
+      <c r="Q14" s="57"/>
     </row>
     <row r="15" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
@@ -1297,12 +1294,12 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="79"/>
-      <c r="M15" s="80"/>
-      <c r="N15" s="81"/>
-      <c r="O15" s="82"/>
-      <c r="P15" s="82"/>
-      <c r="Q15" s="82"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="54"/>
+      <c r="N15" s="55"/>
+      <c r="O15" s="57"/>
+      <c r="P15" s="57"/>
+      <c r="Q15" s="57"/>
     </row>
     <row r="16" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
@@ -1316,12 +1313,12 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="82"/>
-      <c r="M16" s="82"/>
-      <c r="N16" s="82"/>
-      <c r="O16" s="82"/>
-      <c r="P16" s="82"/>
-      <c r="Q16" s="82"/>
+      <c r="L16" s="57"/>
+      <c r="M16" s="57"/>
+      <c r="N16" s="57"/>
+      <c r="O16" s="57"/>
+      <c r="P16" s="57"/>
+      <c r="Q16" s="57"/>
     </row>
     <row r="17" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
@@ -1335,12 +1332,12 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="79"/>
-      <c r="M17" s="80"/>
-      <c r="N17" s="81"/>
-      <c r="O17" s="82"/>
-      <c r="P17" s="82"/>
-      <c r="Q17" s="82"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="54"/>
+      <c r="N17" s="55"/>
+      <c r="O17" s="57"/>
+      <c r="P17" s="57"/>
+      <c r="Q17" s="57"/>
     </row>
     <row r="18" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
@@ -1362,34 +1359,34 @@
       <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="102" t="s">
+      <c r="A19" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="82" t="s">
+      <c r="B19" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="82" t="s">
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="82"/>
-      <c r="I19" s="82"/>
-      <c r="J19" s="82"/>
-      <c r="K19" s="82"/>
-      <c r="L19" s="82" t="s">
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="57"/>
+      <c r="K19" s="57"/>
+      <c r="L19" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="82"/>
-      <c r="N19" s="82"/>
-      <c r="O19" s="82"/>
-      <c r="P19" s="82"/>
-      <c r="Q19" s="82"/>
+      <c r="M19" s="57"/>
+      <c r="N19" s="57"/>
+      <c r="O19" s="57"/>
+      <c r="P19" s="57"/>
+      <c r="Q19" s="57"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="102"/>
+      <c r="A20" s="56"/>
       <c r="B20" s="24" t="s">
         <v>33</v>
       </c>
@@ -1416,25 +1413,25 @@
       </c>
     </row>
     <row r="21" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="64"/>
-      <c r="C21" s="64"/>
-      <c r="D21" s="64"/>
-      <c r="E21" s="64"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="64"/>
-      <c r="H21" s="64"/>
-      <c r="I21" s="64"/>
-      <c r="J21" s="64"/>
-      <c r="K21" s="64"/>
-      <c r="L21" s="64"/>
-      <c r="M21" s="64"/>
-      <c r="N21" s="64"/>
-      <c r="O21" s="64"/>
-      <c r="P21" s="64"/>
-      <c r="Q21" s="62"/>
+      <c r="B21" s="46"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="46"/>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
+      <c r="L21" s="46"/>
+      <c r="M21" s="46"/>
+      <c r="N21" s="46"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="44"/>
     </row>
     <row r="22" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
@@ -1457,7 +1454,7 @@
     </row>
     <row r="23" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="21"/>
-      <c r="C23" s="65" t="s">
+      <c r="C23" s="47" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="23"/>
@@ -1479,9 +1476,9 @@
     </row>
     <row r="24" spans="1:17" s="3" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="78"/>
-      <c r="F24" s="78"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="51"/>
+      <c r="F24" s="51"/>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
@@ -1496,12 +1493,12 @@
     <row r="25" spans="1:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="65" t="s">
+      <c r="C25" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="75"/>
-      <c r="E25" s="76"/>
-      <c r="F25" s="77"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="49"/>
+      <c r="F25" s="50"/>
       <c r="G25" s="22" t="s">
         <v>27</v>
       </c>
@@ -1539,22 +1536,22 @@
   <dimension ref="A1:AP100"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="58" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="58" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="58" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="58" customWidth="1"/>
-    <col min="5" max="10" width="9.5703125" style="58" customWidth="1"/>
-    <col min="11" max="11" width="9" style="58" hidden="1" customWidth="1"/>
-    <col min="12" max="17" width="9.5703125" style="58" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="58"/>
+    <col min="1" max="1" width="4.28515625" style="81" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="81" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="81" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="81" customWidth="1"/>
+    <col min="5" max="10" width="9.5703125" style="81" customWidth="1"/>
+    <col min="11" max="11" width="9" style="81" hidden="1" customWidth="1"/>
+    <col min="12" max="17" width="9.5703125" style="81" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="81"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M1" s="26" t="s">
         <v>8</v>
       </c>
@@ -1563,54 +1560,53 @@
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
       <c r="R1" s="12"/>
-      <c r="S1" s="15"/>
       <c r="T1" s="16"/>
-      <c r="U1" s="42"/>
-      <c r="V1" s="42"/>
-      <c r="W1" s="87"/>
-      <c r="X1" s="87"/>
-      <c r="Y1" s="87"/>
-      <c r="Z1" s="87"/>
-      <c r="AA1" s="87"/>
-      <c r="AB1" s="87"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="62"/>
+      <c r="AA1" s="62"/>
+      <c r="AB1" s="62"/>
       <c r="AC1" s="25"/>
       <c r="AD1" s="17"/>
-      <c r="AE1" s="43"/>
-      <c r="AF1" s="43"/>
-      <c r="AG1" s="43"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="45"/>
-      <c r="AJ1" s="18"/>
-    </row>
-    <row r="2" spans="1:42" s="41" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE1" s="34"/>
+      <c r="AF1" s="34"/>
+      <c r="AG1" s="34"/>
+      <c r="AH1" s="35"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="66"/>
+    </row>
+    <row r="2" spans="1:42" s="15" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="46"/>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="46"/>
-      <c r="S2" s="46"/>
-      <c r="T2" s="46"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="87"/>
-      <c r="X2" s="87"/>
-      <c r="Y2" s="87"/>
-      <c r="Z2" s="87"/>
-      <c r="AA2" s="87"/>
-      <c r="AB2" s="87"/>
-      <c r="AC2" s="87"/>
-      <c r="AD2" s="87"/>
-      <c r="AE2" s="43"/>
-      <c r="AF2" s="43"/>
-      <c r="AG2" s="43"/>
-      <c r="AH2" s="44"/>
-      <c r="AI2" s="45"/>
-      <c r="AJ2" s="18"/>
-    </row>
-    <row r="3" spans="1:42" s="41" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N2" s="37"/>
+      <c r="O2" s="37"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
+      <c r="R2" s="37"/>
+      <c r="S2" s="37"/>
+      <c r="T2" s="37"/>
+      <c r="U2" s="33"/>
+      <c r="V2" s="33"/>
+      <c r="W2" s="62"/>
+      <c r="X2" s="62"/>
+      <c r="Y2" s="62"/>
+      <c r="Z2" s="62"/>
+      <c r="AA2" s="62"/>
+      <c r="AB2" s="62"/>
+      <c r="AC2" s="62"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="34"/>
+      <c r="AF2" s="34"/>
+      <c r="AG2" s="34"/>
+      <c r="AH2" s="35"/>
+      <c r="AI2" s="36"/>
+      <c r="AJ2" s="66"/>
+    </row>
+    <row r="3" spans="1:42" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M3" s="27" t="s">
         <v>37</v>
       </c>
@@ -1621,24 +1617,24 @@
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
-      <c r="U3" s="42"/>
-      <c r="V3" s="42"/>
-      <c r="W3" s="88"/>
-      <c r="X3" s="88"/>
-      <c r="Y3" s="88"/>
-      <c r="Z3" s="88"/>
-      <c r="AA3" s="88"/>
-      <c r="AB3" s="88"/>
-      <c r="AC3" s="88"/>
-      <c r="AD3" s="88"/>
-      <c r="AE3" s="47"/>
-      <c r="AF3" s="47"/>
-      <c r="AG3" s="47"/>
-      <c r="AH3" s="48"/>
-      <c r="AI3" s="48"/>
-      <c r="AJ3" s="18"/>
-    </row>
-    <row r="4" spans="1:42" s="41" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U3" s="33"/>
+      <c r="V3" s="33"/>
+      <c r="W3" s="63"/>
+      <c r="X3" s="63"/>
+      <c r="Y3" s="63"/>
+      <c r="Z3" s="63"/>
+      <c r="AA3" s="63"/>
+      <c r="AB3" s="63"/>
+      <c r="AC3" s="63"/>
+      <c r="AD3" s="63"/>
+      <c r="AE3" s="38"/>
+      <c r="AF3" s="38"/>
+      <c r="AG3" s="38"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="66"/>
+    </row>
+    <row r="4" spans="1:42" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M4" s="26" t="s">
         <v>38</v>
       </c>
@@ -1648,46 +1644,45 @@
       <c r="Q4" s="12"/>
       <c r="R4" s="12"/>
       <c r="S4" s="12"/>
-      <c r="T4" s="15"/>
-      <c r="U4" s="42"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="87"/>
-      <c r="X4" s="87"/>
-      <c r="Y4" s="87"/>
-      <c r="Z4" s="87"/>
-      <c r="AA4" s="87"/>
-      <c r="AB4" s="87"/>
-      <c r="AC4" s="87"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="33"/>
+      <c r="W4" s="62"/>
+      <c r="X4" s="62"/>
+      <c r="Y4" s="62"/>
+      <c r="Z4" s="62"/>
+      <c r="AA4" s="62"/>
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="62"/>
       <c r="AD4" s="25"/>
-      <c r="AE4" s="47"/>
-      <c r="AF4" s="47"/>
-      <c r="AG4" s="47"/>
-      <c r="AH4" s="48"/>
-      <c r="AI4" s="49"/>
-      <c r="AJ4" s="18"/>
-    </row>
-    <row r="5" spans="1:42" s="41" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AE4" s="38"/>
+      <c r="AF4" s="38"/>
+      <c r="AG4" s="38"/>
+      <c r="AH4" s="39"/>
+      <c r="AI4" s="40"/>
+      <c r="AJ4" s="66"/>
+    </row>
+    <row r="5" spans="1:42" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="90"/>
-      <c r="U5" s="90"/>
-      <c r="V5" s="90"/>
-      <c r="W5" s="90"/>
-      <c r="X5" s="90"/>
-      <c r="Y5" s="90"/>
-      <c r="Z5" s="18"/>
-      <c r="AB5" s="42"/>
-      <c r="AC5" s="42"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="91"/>
-      <c r="AF5" s="91"/>
-      <c r="AG5" s="91"/>
-      <c r="AH5" s="91"/>
-      <c r="AI5" s="91"/>
-      <c r="AJ5" s="18"/>
-    </row>
-    <row r="6" spans="1:42" s="41" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T5" s="64"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64"/>
+      <c r="W5" s="64"/>
+      <c r="X5" s="64"/>
+      <c r="Y5" s="64"/>
+      <c r="Z5" s="66"/>
+      <c r="AB5" s="33"/>
+      <c r="AC5" s="33"/>
+      <c r="AD5" s="65"/>
+      <c r="AE5" s="65"/>
+      <c r="AF5" s="65"/>
+      <c r="AG5" s="65"/>
+      <c r="AH5" s="65"/>
+      <c r="AI5" s="65"/>
+      <c r="AJ5" s="66"/>
+    </row>
+    <row r="6" spans="1:42" s="15" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M6" s="30"/>
       <c r="N6" s="19"/>
       <c r="O6" s="19"/>
@@ -1702,24 +1697,24 @@
       <c r="V6" s="17"/>
       <c r="W6" s="25"/>
       <c r="X6" s="25"/>
-      <c r="Y6" s="50"/>
+      <c r="Y6" s="41"/>
       <c r="Z6" s="25"/>
       <c r="AA6" s="17"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="42"/>
+      <c r="AB6" s="33"/>
+      <c r="AC6" s="33"/>
       <c r="AD6" s="17"/>
       <c r="AE6" s="17"/>
       <c r="AF6" s="17"/>
       <c r="AG6" s="25"/>
       <c r="AH6" s="25"/>
-      <c r="AI6" s="50"/>
-      <c r="AL6" s="18"/>
-      <c r="AM6" s="18"/>
-      <c r="AN6" s="18"/>
-      <c r="AO6" s="18"/>
-      <c r="AP6" s="18"/>
-    </row>
-    <row r="7" spans="1:42" s="41" customFormat="1" ht="18" x14ac:dyDescent="0.25">
+      <c r="AI6" s="41"/>
+      <c r="AL6" s="66"/>
+      <c r="AM6" s="66"/>
+      <c r="AN6" s="66"/>
+      <c r="AO6" s="66"/>
+      <c r="AP6" s="66"/>
+    </row>
+    <row r="7" spans="1:42" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="M7" s="32" t="s">
         <v>39</v>
       </c>
@@ -1728,260 +1723,260 @@
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="20"/>
-      <c r="S7" s="18"/>
+      <c r="S7" s="66"/>
       <c r="T7" s="17"/>
-      <c r="U7" s="42"/>
-      <c r="V7" s="42"/>
-      <c r="W7" s="51"/>
-      <c r="X7" s="51"/>
-      <c r="Y7" s="52"/>
-      <c r="Z7" s="52"/>
-      <c r="AA7" s="52"/>
-      <c r="AB7" s="51"/>
-      <c r="AC7" s="51"/>
-      <c r="AD7" s="52"/>
-      <c r="AE7" s="52"/>
-      <c r="AF7" s="52"/>
-      <c r="AG7" s="52"/>
-      <c r="AH7" s="45"/>
-      <c r="AI7" s="45"/>
-      <c r="AL7" s="53"/>
-      <c r="AM7" s="53"/>
-      <c r="AN7" s="53"/>
-    </row>
-    <row r="8" spans="1:42" s="54" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="92" t="s">
+      <c r="U7" s="33"/>
+      <c r="V7" s="33"/>
+      <c r="W7" s="42"/>
+      <c r="X7" s="42"/>
+      <c r="Y7" s="43"/>
+      <c r="Z7" s="43"/>
+      <c r="AA7" s="43"/>
+      <c r="AB7" s="42"/>
+      <c r="AC7" s="42"/>
+      <c r="AD7" s="43"/>
+      <c r="AE7" s="43"/>
+      <c r="AF7" s="43"/>
+      <c r="AG7" s="43"/>
+      <c r="AH7" s="36"/>
+      <c r="AI7" s="36"/>
+      <c r="AL7" s="67"/>
+      <c r="AM7" s="67"/>
+      <c r="AN7" s="67"/>
+    </row>
+    <row r="8" spans="1:42" s="69" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="92"/>
-      <c r="C8" s="92"/>
-      <c r="D8" s="92"/>
-      <c r="E8" s="92"/>
-      <c r="F8" s="92"/>
-      <c r="G8" s="92"/>
-      <c r="H8" s="92"/>
-      <c r="I8" s="92"/>
-      <c r="J8" s="92"/>
-      <c r="K8" s="92"/>
-      <c r="L8" s="92"/>
-      <c r="M8" s="92"/>
-      <c r="N8" s="92"/>
-      <c r="O8" s="92"/>
-      <c r="P8" s="92"/>
-      <c r="Q8" s="92"/>
-    </row>
-    <row r="9" spans="1:42" s="55" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="89" t="s">
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
+    </row>
+    <row r="9" spans="1:42" s="71" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="89"/>
-      <c r="C9" s="89"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="89"/>
-      <c r="F9" s="89"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="89"/>
-      <c r="I9" s="89"/>
-      <c r="J9" s="89"/>
-      <c r="K9" s="89"/>
-      <c r="L9" s="89"/>
-      <c r="M9" s="89"/>
-      <c r="N9" s="89"/>
-      <c r="O9" s="89"/>
-      <c r="P9" s="89"/>
-      <c r="Q9" s="89"/>
-    </row>
-    <row r="10" spans="1:42" s="55" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A10" s="86" t="s">
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="70"/>
+      <c r="G9" s="70"/>
+      <c r="H9" s="70"/>
+      <c r="I9" s="70"/>
+      <c r="J9" s="70"/>
+      <c r="K9" s="70"/>
+      <c r="L9" s="70"/>
+      <c r="M9" s="70"/>
+      <c r="N9" s="70"/>
+      <c r="O9" s="70"/>
+      <c r="P9" s="70"/>
+      <c r="Q9" s="70"/>
+    </row>
+    <row r="10" spans="1:42" s="71" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="86"/>
-      <c r="C10" s="86"/>
-      <c r="D10" s="86"/>
-      <c r="E10" s="86"/>
-      <c r="F10" s="86"/>
-      <c r="G10" s="86"/>
-      <c r="H10" s="86"/>
-      <c r="I10" s="86"/>
-      <c r="J10" s="86"/>
-      <c r="K10" s="86"/>
-      <c r="L10" s="86"/>
-      <c r="M10" s="86"/>
-      <c r="N10" s="86"/>
-      <c r="O10" s="86"/>
-      <c r="P10" s="86"/>
-      <c r="Q10" s="86"/>
-    </row>
-    <row r="11" spans="1:42" s="41" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="56"/>
-      <c r="B11" s="56"/>
-      <c r="C11" s="56"/>
-      <c r="D11" s="56"/>
-      <c r="E11" s="56"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-      <c r="H11" s="56"/>
-      <c r="I11" s="56"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="103" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="61"/>
+      <c r="I10" s="61"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="61"/>
+      <c r="L10" s="61"/>
+      <c r="M10" s="61"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="61"/>
+    </row>
+    <row r="11" spans="1:42" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="72"/>
+      <c r="B11" s="72"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="72"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="72"/>
+      <c r="J11" s="72"/>
+      <c r="K11" s="72"/>
+      <c r="L11" s="72"/>
+      <c r="M11" s="72"/>
+      <c r="O11" s="73"/>
+      <c r="P11" s="73"/>
+      <c r="Q11" s="74" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:42" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="93" t="s">
+      <c r="A12" s="75" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="95" t="s">
+      <c r="B12" s="76" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="96" t="s">
+      <c r="C12" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="76" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="97" t="s">
+      <c r="E12" s="78" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
-      <c r="I12" s="98"/>
-      <c r="J12" s="98"/>
-      <c r="K12" s="99"/>
-      <c r="L12" s="96" t="s">
+      <c r="F12" s="79"/>
+      <c r="G12" s="79"/>
+      <c r="H12" s="79"/>
+      <c r="I12" s="79"/>
+      <c r="J12" s="79"/>
+      <c r="K12" s="80"/>
+      <c r="L12" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="96"/>
-      <c r="N12" s="96"/>
-      <c r="O12" s="96"/>
-      <c r="P12" s="96"/>
-      <c r="Q12" s="96"/>
+      <c r="M12" s="77"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="77"/>
+      <c r="P12" s="77"/>
+      <c r="Q12" s="77"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A13" s="94"/>
-      <c r="B13" s="100"/>
-      <c r="C13" s="101"/>
-      <c r="D13" s="100"/>
-      <c r="E13" s="33" t="s">
+      <c r="A13" s="82"/>
+      <c r="B13" s="83"/>
+      <c r="C13" s="84"/>
+      <c r="D13" s="83"/>
+      <c r="E13" s="85" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="33"/>
-      <c r="G13" s="33"/>
-      <c r="H13" s="33"/>
-      <c r="I13" s="33"/>
-      <c r="J13" s="33" t="s">
+      <c r="F13" s="85"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="85"/>
+      <c r="I13" s="85"/>
+      <c r="J13" s="85" t="s">
         <v>0</v>
       </c>
-      <c r="K13" s="33" t="s">
+      <c r="K13" s="85" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="33" t="s">
+      <c r="L13" s="85" t="s">
         <v>36</v>
       </c>
-      <c r="M13" s="33"/>
-      <c r="N13" s="33"/>
-      <c r="O13" s="33"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33" t="s">
+      <c r="M13" s="85"/>
+      <c r="N13" s="85"/>
+      <c r="O13" s="85"/>
+      <c r="P13" s="85"/>
+      <c r="Q13" s="85" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="86" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="73"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="73"/>
-      <c r="H14" s="73"/>
-      <c r="I14" s="73"/>
-      <c r="J14" s="73"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="73"/>
-      <c r="N14" s="73"/>
-      <c r="O14" s="73"/>
-      <c r="P14" s="73"/>
-      <c r="Q14" s="73"/>
-    </row>
-    <row r="15" spans="1:42" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="61"/>
-      <c r="N15" s="61"/>
-      <c r="O15" s="61"/>
-      <c r="P15" s="61"/>
-      <c r="Q15" s="61"/>
-    </row>
-    <row r="16" spans="1:42" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="59"/>
-      <c r="B16" s="59"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="59"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="61"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="61"/>
-      <c r="J16" s="61"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="61"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="61"/>
-      <c r="P16" s="61"/>
-      <c r="Q16" s="61"/>
-    </row>
-    <row r="17" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="68"/>
-      <c r="C17" s="67" t="s">
+      <c r="B14" s="86"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="88"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="52"/>
+      <c r="P14" s="52"/>
+      <c r="Q14" s="52"/>
+    </row>
+    <row r="15" spans="1:42" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="89"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="90"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="91"/>
+      <c r="G15" s="91"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="91"/>
+      <c r="K15" s="91"/>
+      <c r="L15" s="91"/>
+      <c r="M15" s="91"/>
+      <c r="N15" s="91"/>
+      <c r="O15" s="91"/>
+      <c r="P15" s="91"/>
+      <c r="Q15" s="91"/>
+    </row>
+    <row r="16" spans="1:42" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="89"/>
+      <c r="B16" s="89"/>
+      <c r="C16" s="90"/>
+      <c r="D16" s="89"/>
+      <c r="E16" s="91"/>
+      <c r="F16" s="91"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="91"/>
+      <c r="J16" s="91"/>
+      <c r="K16" s="91"/>
+      <c r="L16" s="91"/>
+      <c r="M16" s="91"/>
+      <c r="N16" s="91"/>
+      <c r="O16" s="91"/>
+      <c r="P16" s="91"/>
+      <c r="Q16" s="91"/>
+    </row>
+    <row r="17" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="92"/>
+      <c r="C17" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="36"/>
-      <c r="E17" s="36"/>
-      <c r="F17" s="37" t="s">
+      <c r="D17" s="94"/>
+      <c r="E17" s="94"/>
+      <c r="F17" s="95" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="34"/>
-    </row>
-    <row r="18" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="69"/>
-      <c r="F18" s="40"/>
-      <c r="G18" s="35"/>
-    </row>
-    <row r="19" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="66" t="s">
+      <c r="G17" s="96"/>
+    </row>
+    <row r="18" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="97"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="99"/>
+    </row>
+    <row r="19" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="100" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="38"/>
-      <c r="E19" s="39"/>
-    </row>
-    <row r="20" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:7" s="41" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D19" s="101"/>
+      <c r="E19" s="102"/>
+    </row>
+    <row r="20" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2058,6 +2053,12 @@
     <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="L12:Q12"/>
+    <mergeCell ref="E12:K12"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
     <mergeCell ref="W1:AB1"/>
     <mergeCell ref="W2:AD2"/>
     <mergeCell ref="W3:AD3"/>
@@ -2067,12 +2068,6 @@
     <mergeCell ref="AD5:AI5"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="A8:Q8"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="L12:Q12"/>
-    <mergeCell ref="E12:K12"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.31496062992125984" top="0.78740157480314965" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="83" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>

<commit_message>
increase row height, font size
</commit_message>
<xml_diff>
--- a/spreadsheets/menu_report.xlsx
+++ b/spreadsheets/menu_report.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ЦяКнига" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="19440" windowHeight="13875"/>
@@ -529,55 +529,9 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -587,42 +541,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -656,9 +577,88 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Звичайний" xfId="0" builtinId="0"/>
     <cellStyle name="Обычный 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -677,7 +677,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Стандартна">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -715,7 +715,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Стандартна">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -787,7 +787,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Стандартна">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1135,46 +1135,46 @@
       <c r="Q7" s="18"/>
     </row>
     <row r="8" spans="1:17" s="10" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="59"/>
-      <c r="C8" s="59"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="59"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="59"/>
-      <c r="J8" s="59"/>
-      <c r="K8" s="59"/>
-      <c r="L8" s="59"/>
-      <c r="M8" s="59"/>
-      <c r="N8" s="59"/>
-      <c r="O8" s="59"/>
-      <c r="P8" s="59"/>
-      <c r="Q8" s="59"/>
+      <c r="B8" s="76"/>
+      <c r="C8" s="76"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76"/>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="76"/>
+      <c r="K8" s="76"/>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="76"/>
+      <c r="O8" s="76"/>
+      <c r="P8" s="76"/>
+      <c r="Q8" s="76"/>
     </row>
     <row r="9" spans="1:17" s="9" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="61"/>
-      <c r="J9" s="61"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="61"/>
-      <c r="N9" s="61"/>
-      <c r="O9" s="61"/>
-      <c r="P9" s="61"/>
-      <c r="Q9" s="61"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82"/>
+      <c r="D9" s="82"/>
+      <c r="E9" s="82"/>
+      <c r="F9" s="82"/>
+      <c r="G9" s="82"/>
+      <c r="H9" s="82"/>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="82"/>
+      <c r="Q9" s="82"/>
     </row>
     <row r="10" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A10" s="8"/>
@@ -1207,14 +1207,14 @@
       <c r="I11" s="8"/>
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
-      <c r="L11" s="60" t="s">
+      <c r="L11" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="M11" s="60"/>
-      <c r="N11" s="60"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="60"/>
+      <c r="M11" s="81"/>
+      <c r="N11" s="81"/>
+      <c r="O11" s="81"/>
+      <c r="P11" s="81"/>
+      <c r="Q11" s="81"/>
     </row>
     <row r="12" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
@@ -1228,17 +1228,17 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
-      <c r="L12" s="57" t="s">
+      <c r="L12" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="M12" s="57"/>
-      <c r="N12" s="57"/>
-      <c r="O12" s="57">
+      <c r="M12" s="77"/>
+      <c r="N12" s="77"/>
+      <c r="O12" s="77">
         <f>SUM(O13:Q17)</f>
         <v>0</v>
       </c>
-      <c r="P12" s="58"/>
-      <c r="Q12" s="58"/>
+      <c r="P12" s="83"/>
+      <c r="Q12" s="83"/>
     </row>
     <row r="13" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="8"/>
@@ -1252,16 +1252,16 @@
       <c r="I13" s="8"/>
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
-      <c r="L13" s="53" t="s">
+      <c r="L13" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="M13" s="54"/>
-      <c r="N13" s="55"/>
-      <c r="O13" s="57" t="s">
+      <c r="M13" s="79"/>
+      <c r="N13" s="80"/>
+      <c r="O13" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="P13" s="58"/>
-      <c r="Q13" s="58"/>
+      <c r="P13" s="83"/>
+      <c r="Q13" s="83"/>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
@@ -1275,12 +1275,12 @@
       <c r="I14" s="8"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="55"/>
-      <c r="O14" s="57"/>
-      <c r="P14" s="57"/>
-      <c r="Q14" s="57"/>
+      <c r="L14" s="78"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="80"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77"/>
+      <c r="Q14" s="77"/>
     </row>
     <row r="15" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="8"/>
@@ -1294,12 +1294,12 @@
       <c r="I15" s="8"/>
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
-      <c r="L15" s="53"/>
-      <c r="M15" s="54"/>
-      <c r="N15" s="55"/>
-      <c r="O15" s="57"/>
-      <c r="P15" s="57"/>
-      <c r="Q15" s="57"/>
+      <c r="L15" s="78"/>
+      <c r="M15" s="79"/>
+      <c r="N15" s="80"/>
+      <c r="O15" s="77"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="77"/>
     </row>
     <row r="16" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="8"/>
@@ -1313,12 +1313,12 @@
       <c r="I16" s="8"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="57"/>
+      <c r="L16" s="77"/>
+      <c r="M16" s="77"/>
+      <c r="N16" s="77"/>
+      <c r="O16" s="77"/>
+      <c r="P16" s="77"/>
+      <c r="Q16" s="77"/>
     </row>
     <row r="17" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A17" s="8"/>
@@ -1332,12 +1332,12 @@
       <c r="I17" s="8"/>
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
-      <c r="L17" s="53"/>
-      <c r="M17" s="54"/>
-      <c r="N17" s="55"/>
-      <c r="O17" s="57"/>
-      <c r="P17" s="57"/>
-      <c r="Q17" s="57"/>
+      <c r="L17" s="78"/>
+      <c r="M17" s="79"/>
+      <c r="N17" s="80"/>
+      <c r="O17" s="77"/>
+      <c r="P17" s="77"/>
+      <c r="Q17" s="77"/>
     </row>
     <row r="18" spans="1:17" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="8"/>
@@ -1359,34 +1359,34 @@
       <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="56" t="s">
+      <c r="A19" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="77" t="s">
         <v>3</v>
       </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57" t="s">
+      <c r="C19" s="77"/>
+      <c r="D19" s="77"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77" t="s">
         <v>2</v>
       </c>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57" t="s">
+      <c r="H19" s="77"/>
+      <c r="I19" s="77"/>
+      <c r="J19" s="77"/>
+      <c r="K19" s="77"/>
+      <c r="L19" s="77" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="57"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="57"/>
-      <c r="P19" s="57"/>
-      <c r="Q19" s="57"/>
+      <c r="M19" s="77"/>
+      <c r="N19" s="77"/>
+      <c r="O19" s="77"/>
+      <c r="P19" s="77"/>
+      <c r="Q19" s="77"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" s="56"/>
+      <c r="A20" s="84"/>
       <c r="B20" s="24" t="s">
         <v>33</v>
       </c>
@@ -1505,6 +1505,9 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="O16:Q16"/>
+    <mergeCell ref="O17:Q17"/>
+    <mergeCell ref="L16:N16"/>
     <mergeCell ref="A8:Q8"/>
     <mergeCell ref="B19:F19"/>
     <mergeCell ref="L17:N17"/>
@@ -1521,9 +1524,6 @@
     <mergeCell ref="L14:N14"/>
     <mergeCell ref="A19:A20"/>
     <mergeCell ref="O12:Q12"/>
-    <mergeCell ref="O16:Q16"/>
-    <mergeCell ref="O17:Q17"/>
-    <mergeCell ref="L16:N16"/>
   </mergeCells>
   <pageMargins left="0.56000000000000005" right="0.37" top="0.62" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="74" fitToHeight="0" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
@@ -1536,19 +1536,19 @@
   <dimension ref="A1:AP100"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="81" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" style="81" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="81" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="81" customWidth="1"/>
-    <col min="5" max="10" width="9.5703125" style="81" customWidth="1"/>
-    <col min="11" max="11" width="9" style="81" hidden="1" customWidth="1"/>
-    <col min="12" max="17" width="9.5703125" style="81" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="81"/>
+    <col min="1" max="1" width="4.28515625" style="60" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" style="60" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" style="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="60" customWidth="1"/>
+    <col min="5" max="10" width="9.5703125" style="60" customWidth="1"/>
+    <col min="11" max="11" width="9" style="60" hidden="1" customWidth="1"/>
+    <col min="12" max="17" width="9.5703125" style="60" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="60"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:42" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1563,12 +1563,12 @@
       <c r="T1" s="16"/>
       <c r="U1" s="33"/>
       <c r="V1" s="33"/>
-      <c r="W1" s="62"/>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62"/>
-      <c r="AB1" s="62"/>
+      <c r="W1" s="94"/>
+      <c r="X1" s="94"/>
+      <c r="Y1" s="94"/>
+      <c r="Z1" s="94"/>
+      <c r="AA1" s="94"/>
+      <c r="AB1" s="94"/>
       <c r="AC1" s="25"/>
       <c r="AD1" s="17"/>
       <c r="AE1" s="34"/>
@@ -1576,7 +1576,7 @@
       <c r="AG1" s="34"/>
       <c r="AH1" s="35"/>
       <c r="AI1" s="36"/>
-      <c r="AJ1" s="66"/>
+      <c r="AJ1" s="52"/>
     </row>
     <row r="2" spans="1:42" s="15" customFormat="1" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M2" s="26" t="s">
@@ -1591,20 +1591,20 @@
       <c r="T2" s="37"/>
       <c r="U2" s="33"/>
       <c r="V2" s="33"/>
-      <c r="W2" s="62"/>
-      <c r="X2" s="62"/>
-      <c r="Y2" s="62"/>
-      <c r="Z2" s="62"/>
-      <c r="AA2" s="62"/>
-      <c r="AB2" s="62"/>
-      <c r="AC2" s="62"/>
-      <c r="AD2" s="62"/>
+      <c r="W2" s="94"/>
+      <c r="X2" s="94"/>
+      <c r="Y2" s="94"/>
+      <c r="Z2" s="94"/>
+      <c r="AA2" s="94"/>
+      <c r="AB2" s="94"/>
+      <c r="AC2" s="94"/>
+      <c r="AD2" s="94"/>
       <c r="AE2" s="34"/>
       <c r="AF2" s="34"/>
       <c r="AG2" s="34"/>
       <c r="AH2" s="35"/>
       <c r="AI2" s="36"/>
-      <c r="AJ2" s="66"/>
+      <c r="AJ2" s="52"/>
     </row>
     <row r="3" spans="1:42" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M3" s="27" t="s">
@@ -1619,20 +1619,20 @@
       <c r="T3" s="13"/>
       <c r="U3" s="33"/>
       <c r="V3" s="33"/>
-      <c r="W3" s="63"/>
-      <c r="X3" s="63"/>
-      <c r="Y3" s="63"/>
-      <c r="Z3" s="63"/>
-      <c r="AA3" s="63"/>
-      <c r="AB3" s="63"/>
-      <c r="AC3" s="63"/>
-      <c r="AD3" s="63"/>
+      <c r="W3" s="95"/>
+      <c r="X3" s="95"/>
+      <c r="Y3" s="95"/>
+      <c r="Z3" s="95"/>
+      <c r="AA3" s="95"/>
+      <c r="AB3" s="95"/>
+      <c r="AC3" s="95"/>
+      <c r="AD3" s="95"/>
       <c r="AE3" s="38"/>
       <c r="AF3" s="38"/>
       <c r="AG3" s="38"/>
       <c r="AH3" s="39"/>
       <c r="AI3" s="39"/>
-      <c r="AJ3" s="66"/>
+      <c r="AJ3" s="52"/>
     </row>
     <row r="4" spans="1:42" s="15" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M4" s="26" t="s">
@@ -1646,41 +1646,41 @@
       <c r="S4" s="12"/>
       <c r="U4" s="33"/>
       <c r="V4" s="33"/>
-      <c r="W4" s="62"/>
-      <c r="X4" s="62"/>
-      <c r="Y4" s="62"/>
-      <c r="Z4" s="62"/>
-      <c r="AA4" s="62"/>
-      <c r="AB4" s="62"/>
-      <c r="AC4" s="62"/>
+      <c r="W4" s="94"/>
+      <c r="X4" s="94"/>
+      <c r="Y4" s="94"/>
+      <c r="Z4" s="94"/>
+      <c r="AA4" s="94"/>
+      <c r="AB4" s="94"/>
+      <c r="AC4" s="94"/>
       <c r="AD4" s="25"/>
       <c r="AE4" s="38"/>
       <c r="AF4" s="38"/>
       <c r="AG4" s="38"/>
       <c r="AH4" s="39"/>
       <c r="AI4" s="40"/>
-      <c r="AJ4" s="66"/>
+      <c r="AJ4" s="52"/>
     </row>
     <row r="5" spans="1:42" s="15" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M5" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="64"/>
-      <c r="Z5" s="66"/>
+      <c r="T5" s="97"/>
+      <c r="U5" s="97"/>
+      <c r="V5" s="97"/>
+      <c r="W5" s="97"/>
+      <c r="X5" s="97"/>
+      <c r="Y5" s="97"/>
+      <c r="Z5" s="52"/>
       <c r="AB5" s="33"/>
       <c r="AC5" s="33"/>
-      <c r="AD5" s="65"/>
-      <c r="AE5" s="65"/>
-      <c r="AF5" s="65"/>
-      <c r="AG5" s="65"/>
-      <c r="AH5" s="65"/>
-      <c r="AI5" s="65"/>
-      <c r="AJ5" s="66"/>
+      <c r="AD5" s="98"/>
+      <c r="AE5" s="98"/>
+      <c r="AF5" s="98"/>
+      <c r="AG5" s="98"/>
+      <c r="AH5" s="98"/>
+      <c r="AI5" s="98"/>
+      <c r="AJ5" s="52"/>
     </row>
     <row r="6" spans="1:42" s="15" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M6" s="30"/>
@@ -1708,11 +1708,11 @@
       <c r="AG6" s="25"/>
       <c r="AH6" s="25"/>
       <c r="AI6" s="41"/>
-      <c r="AL6" s="66"/>
-      <c r="AM6" s="66"/>
-      <c r="AN6" s="66"/>
-      <c r="AO6" s="66"/>
-      <c r="AP6" s="66"/>
+      <c r="AL6" s="52"/>
+      <c r="AM6" s="52"/>
+      <c r="AN6" s="52"/>
+      <c r="AO6" s="52"/>
+      <c r="AP6" s="52"/>
     </row>
     <row r="7" spans="1:42" s="15" customFormat="1" ht="18" x14ac:dyDescent="0.25">
       <c r="M7" s="32" t="s">
@@ -1723,7 +1723,7 @@
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="20"/>
-      <c r="S7" s="66"/>
+      <c r="S7" s="52"/>
       <c r="T7" s="17"/>
       <c r="U7" s="33"/>
       <c r="V7" s="33"/>
@@ -1740,325 +1740,319 @@
       <c r="AG7" s="43"/>
       <c r="AH7" s="36"/>
       <c r="AI7" s="36"/>
-      <c r="AL7" s="67"/>
-      <c r="AM7" s="67"/>
-      <c r="AN7" s="67"/>
-    </row>
-    <row r="8" spans="1:42" s="69" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="68" t="s">
+      <c r="AL7" s="53"/>
+      <c r="AM7" s="53"/>
+      <c r="AN7" s="53"/>
+    </row>
+    <row r="8" spans="1:42" s="54" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="99" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
-      <c r="J8" s="68"/>
-      <c r="K8" s="68"/>
-      <c r="L8" s="68"/>
-      <c r="M8" s="68"/>
-      <c r="N8" s="68"/>
-      <c r="O8" s="68"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
-    </row>
-    <row r="9" spans="1:42" s="71" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A9" s="70" t="s">
+      <c r="B8" s="99"/>
+      <c r="C8" s="99"/>
+      <c r="D8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="99"/>
+      <c r="N8" s="99"/>
+      <c r="O8" s="99"/>
+      <c r="P8" s="99"/>
+      <c r="Q8" s="99"/>
+    </row>
+    <row r="9" spans="1:42" s="55" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A9" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="70"/>
-    </row>
-    <row r="10" spans="1:42" s="71" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A10" s="61" t="s">
+      <c r="B9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="96"/>
+      <c r="G9" s="96"/>
+      <c r="H9" s="96"/>
+      <c r="I9" s="96"/>
+      <c r="J9" s="96"/>
+      <c r="K9" s="96"/>
+      <c r="L9" s="96"/>
+      <c r="M9" s="96"/>
+      <c r="N9" s="96"/>
+      <c r="O9" s="96"/>
+      <c r="P9" s="96"/>
+      <c r="Q9" s="96"/>
+    </row>
+    <row r="10" spans="1:42" s="55" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A10" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="61"/>
-      <c r="F10" s="61"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="61"/>
-      <c r="J10" s="61"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="61"/>
-      <c r="N10" s="61"/>
-      <c r="O10" s="61"/>
-      <c r="P10" s="61"/>
-      <c r="Q10" s="61"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="82"/>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
     </row>
     <row r="11" spans="1:42" s="15" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="72"/>
-      <c r="B11" s="72"/>
-      <c r="C11" s="72"/>
-      <c r="D11" s="72"/>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72"/>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="72"/>
-      <c r="K11" s="72"/>
-      <c r="L11" s="72"/>
-      <c r="M11" s="72"/>
-      <c r="O11" s="73"/>
-      <c r="P11" s="73"/>
-      <c r="Q11" s="74" t="s">
+      <c r="A11" s="56"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="56"/>
+      <c r="M11" s="56"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="58" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:42" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="92" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="76" t="s">
+      <c r="B12" s="87" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="85" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="76" t="s">
+      <c r="D12" s="87" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="78" t="s">
+      <c r="E12" s="89" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="79"/>
-      <c r="G12" s="79"/>
-      <c r="H12" s="79"/>
-      <c r="I12" s="79"/>
-      <c r="J12" s="79"/>
-      <c r="K12" s="80"/>
-      <c r="L12" s="77" t="s">
+      <c r="F12" s="90"/>
+      <c r="G12" s="90"/>
+      <c r="H12" s="90"/>
+      <c r="I12" s="90"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="91"/>
+      <c r="L12" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="M12" s="77"/>
-      <c r="N12" s="77"/>
-      <c r="O12" s="77"/>
-      <c r="P12" s="77"/>
-      <c r="Q12" s="77"/>
+      <c r="M12" s="85"/>
+      <c r="N12" s="85"/>
+      <c r="O12" s="85"/>
+      <c r="P12" s="85"/>
+      <c r="Q12" s="85"/>
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A13" s="82"/>
-      <c r="B13" s="83"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="83"/>
-      <c r="E13" s="85" t="s">
+      <c r="A13" s="93"/>
+      <c r="B13" s="88"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="F13" s="85"/>
-      <c r="G13" s="85"/>
-      <c r="H13" s="85"/>
-      <c r="I13" s="85"/>
-      <c r="J13" s="85" t="s">
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="K13" s="85" t="s">
+      <c r="K13" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="L13" s="85" t="s">
+      <c r="L13" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="M13" s="85"/>
-      <c r="N13" s="85"/>
-      <c r="O13" s="85"/>
-      <c r="P13" s="85"/>
-      <c r="Q13" s="85" t="s">
+      <c r="M13" s="61"/>
+      <c r="N13" s="61"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="61"/>
+      <c r="Q13" s="61" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="86" t="s">
+    <row r="14" spans="1:42" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="100" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="86"/>
-      <c r="C14" s="87"/>
-      <c r="D14" s="88"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="52"/>
-    </row>
-    <row r="15" spans="1:42" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="89"/>
-      <c r="B15" s="89"/>
-      <c r="C15" s="90"/>
-      <c r="D15" s="89"/>
-      <c r="E15" s="91"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="91"/>
-      <c r="H15" s="91"/>
-      <c r="I15" s="91"/>
-      <c r="J15" s="91"/>
-      <c r="K15" s="91"/>
-      <c r="L15" s="91"/>
-      <c r="M15" s="91"/>
-      <c r="N15" s="91"/>
-      <c r="O15" s="91"/>
-      <c r="P15" s="91"/>
-      <c r="Q15" s="91"/>
-    </row>
-    <row r="16" spans="1:42" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="89"/>
-      <c r="B16" s="89"/>
-      <c r="C16" s="90"/>
-      <c r="D16" s="89"/>
-      <c r="E16" s="91"/>
-      <c r="F16" s="91"/>
-      <c r="G16" s="91"/>
-      <c r="H16" s="91"/>
-      <c r="I16" s="91"/>
-      <c r="J16" s="91"/>
-      <c r="K16" s="91"/>
-      <c r="L16" s="91"/>
-      <c r="M16" s="91"/>
-      <c r="N16" s="91"/>
-      <c r="O16" s="91"/>
-      <c r="P16" s="91"/>
-      <c r="Q16" s="91"/>
-    </row>
-    <row r="17" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="92"/>
-      <c r="C17" s="93" t="s">
+      <c r="B14" s="100"/>
+      <c r="C14" s="101"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102"/>
+      <c r="H14" s="102"/>
+      <c r="I14" s="102"/>
+      <c r="J14" s="102"/>
+      <c r="K14" s="102"/>
+      <c r="L14" s="102"/>
+      <c r="M14" s="102"/>
+      <c r="N14" s="102"/>
+      <c r="O14" s="102"/>
+      <c r="P14" s="102"/>
+      <c r="Q14" s="102"/>
+    </row>
+    <row r="15" spans="1:42" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="62"/>
+      <c r="B15" s="62"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="64"/>
+      <c r="G15" s="64"/>
+      <c r="H15" s="64"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="64"/>
+      <c r="L15" s="64"/>
+      <c r="M15" s="64"/>
+      <c r="N15" s="64"/>
+      <c r="O15" s="64"/>
+      <c r="P15" s="64"/>
+      <c r="Q15" s="64"/>
+    </row>
+    <row r="16" spans="1:42" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="62"/>
+      <c r="B16" s="62"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="64"/>
+      <c r="F16" s="64"/>
+      <c r="G16" s="64"/>
+      <c r="H16" s="64"/>
+      <c r="I16" s="64"/>
+      <c r="J16" s="64"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="64"/>
+      <c r="M16" s="64"/>
+      <c r="N16" s="64"/>
+      <c r="O16" s="64"/>
+      <c r="P16" s="64"/>
+      <c r="Q16" s="64"/>
+    </row>
+    <row r="17" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="65"/>
+      <c r="C17" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="94"/>
-      <c r="E17" s="94"/>
-      <c r="F17" s="95" t="s">
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="G17" s="96"/>
-    </row>
-    <row r="18" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="97"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="99"/>
-    </row>
-    <row r="19" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="100" t="s">
+      <c r="G17" s="69"/>
+    </row>
+    <row r="18" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="70"/>
+      <c r="F18" s="71"/>
+      <c r="G18" s="72"/>
+    </row>
+    <row r="19" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="101"/>
-      <c r="E19" s="102"/>
-    </row>
-    <row r="20" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:7" s="15" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="D19" s="74"/>
+      <c r="E19" s="75"/>
+    </row>
+    <row r="20" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:7" s="15" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="2:7" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="49" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="50" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="51" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="52" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="65" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="L12:Q12"/>
-    <mergeCell ref="E12:K12"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
     <mergeCell ref="W1:AB1"/>
     <mergeCell ref="W2:AD2"/>
     <mergeCell ref="W3:AD3"/>
@@ -2068,6 +2062,12 @@
     <mergeCell ref="AD5:AI5"/>
     <mergeCell ref="W4:AC4"/>
     <mergeCell ref="A8:Q8"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="L12:Q12"/>
+    <mergeCell ref="E12:K12"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
   </mergeCells>
   <pageMargins left="0.62992125984251968" right="0.31496062992125984" top="0.78740157480314965" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="83" orientation="landscape" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>